<commit_message>
10/21/2020: Updated QA automation standard guidelines & comments in FDR-Validation-Voucher and Voucher package.
</commit_message>
<xml_diff>
--- a/Data Files/Regression-Voucher/E2E Regression-Data.xlsx
+++ b/Data Files/Regression-Voucher/E2E Regression-Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fdr-automation-develop_08_25_2020\Data Files\Regression-Voucher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FDR-Katalon-Regression\Data Files\Regression-Voucher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B73AF1-1983-4957-9EDD-3B4974B11B9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39FD4817-1561-484D-A895-0272ECAA814D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" activeTab="5" xr2:uid="{0E06ACD6-6E3B-FF4A-9DD5-148BBE59C4CD}"/>
+    <workbookView xWindow="28680" yWindow="-1815" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0E06ACD6-6E3B-FF4A-9DD5-148BBE59C4CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Variables" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Voucher4" sheetId="5" r:id="rId5"/>
     <sheet name="Voucher5" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -919,7 +919,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -932,7 +932,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="29">
-        <v>44102</v>
+        <v>44111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29">
-        <v>44104</v>
+        <v>44113</v>
       </c>
     </row>
   </sheetData>
@@ -953,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521DC52D-8F10-9A44-AA0B-257816EA388F}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -1075,11 +1075,11 @@
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="31">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B2" s="31">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C2" s="24" t="s">
         <v>34</v>
@@ -1180,11 +1180,11 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B3" s="31">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C3" s="24" t="s">
         <v>34</v>
@@ -1282,11 +1282,11 @@
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B4" s="31">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>34</v>
@@ -1387,11 +1387,11 @@
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B5" s="31">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>34</v>
@@ -1622,11 +1622,11 @@
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B2" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -1727,11 +1727,11 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B3" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1829,11 +1829,11 @@
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B4" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -1934,11 +1934,11 @@
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B5" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
@@ -2039,11 +2039,11 @@
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B6" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -2144,11 +2144,11 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B7" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -2246,11 +2246,11 @@
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B8" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -2351,11 +2351,11 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B9" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -2456,11 +2456,11 @@
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B10" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -2561,11 +2561,11 @@
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B11" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -2663,11 +2663,11 @@
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B12" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -2768,11 +2768,11 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B13" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -3029,11 +3029,11 @@
     <row r="2" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B2" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -3134,11 +3134,11 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B3" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -3236,11 +3236,11 @@
     <row r="4" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B4" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -3341,11 +3341,11 @@
     <row r="5" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B5" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
@@ -3446,11 +3446,11 @@
     <row r="6" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B6" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -3551,11 +3551,11 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B7" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -3653,11 +3653,11 @@
     <row r="8" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B8" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -3758,11 +3758,11 @@
     <row r="9" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B9" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -3863,11 +3863,11 @@
     <row r="10" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B10" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -3968,11 +3968,11 @@
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B11" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -4070,11 +4070,11 @@
     <row r="12" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B12" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -4175,11 +4175,11 @@
     <row r="13" spans="1:34" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B13" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -4435,11 +4435,11 @@
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B2" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>34</v>
@@ -4540,11 +4540,11 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B3" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>34</v>
@@ -4645,11 +4645,11 @@
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B4" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>34</v>
@@ -4750,11 +4750,11 @@
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B5" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C5" s="27" t="s">
         <v>34</v>
@@ -4855,11 +4855,11 @@
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B6" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>34</v>
@@ -4960,11 +4960,11 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B7" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>34</v>
@@ -5065,11 +5065,11 @@
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B8" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>34</v>
@@ -5170,11 +5170,11 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B9" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>34</v>
@@ -5275,11 +5275,11 @@
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B10" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>34</v>
@@ -5380,11 +5380,11 @@
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B11" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>34</v>
@@ -5485,11 +5485,11 @@
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="35">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B12" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>34</v>
@@ -5598,7 +5598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36FAA045-7802-454B-A0A6-8879DD540DD4}">
   <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -5746,11 +5746,11 @@
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B2" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -5851,11 +5851,11 @@
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B3" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -5953,11 +5953,11 @@
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B4" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -6058,11 +6058,11 @@
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B5" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
@@ -6163,11 +6163,11 @@
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B6" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -6268,11 +6268,11 @@
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B7" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
@@ -6370,11 +6370,11 @@
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B8" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -6475,11 +6475,11 @@
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B9" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C9" t="s">
         <v>34</v>
@@ -6580,11 +6580,11 @@
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B10" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -6685,11 +6685,11 @@
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B11" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -6787,11 +6787,11 @@
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B12" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -6892,11 +6892,11 @@
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <f>'Global Variables'!B1</f>
-        <v>44102</v>
+        <v>44111</v>
       </c>
       <c r="B13" s="29">
         <f>'Global Variables'!B2</f>
-        <v>44104</v>
+        <v>44113</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>

</xml_diff>